<commit_message>
run the LLM pipeline on GPU
</commit_message>
<xml_diff>
--- a/out/metadata_gemma3_4B.xlsx
+++ b/out/metadata_gemma3_4B.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,43 +469,505 @@
           <t>% cellules</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Qualité du séquençage</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>24EM03355</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>24CU550062-2ebus</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CLP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CurePath</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Carcinome non à petites cellules NOS</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>20%</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>24EM03456</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>24CU052383</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>CLP</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Curepath</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Adénocarcinome TTF1+</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Optimale</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>10%</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>24EM03461</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>24CU002162-4</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>GP</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Curepath</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Adénocarcinome colorectal métastatique</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>20%</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>24EM03462</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>24219576 1.1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>GP</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>CMP</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Métastase hépatique d’un adénocarcinome mammaire</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>24EM03839</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>24EC09559</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>OST</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Erasme</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>PF2</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>24EM04099</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>24CU062291-frottis2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>OST</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>CurePath</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>PF1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
+      <c r="H7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>24EM04107</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>24CU062294-1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>OST</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>CurePath</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>PF1 oncocytaire</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>10%</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>24EM04337</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2431646-1.1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>OST</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>CMP Pathology</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>masse gastrique</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>24EM04347</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>23CU032757-1.02</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>OST</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>CurePath</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>carcinome urothélial invasif</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>24EM03451</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>24BB11466</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>GP</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>HUB – Centre d’Anatomie Pathologique –</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Tumeur de la granulosa</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>30%</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>24EM03460</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>24MH9721 BN</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>GP</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Centre Hospitalier de Mouscron</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Adénocarcinome lieberkühnien</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>24EM03308</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>24218507-1.1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>GP</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>CMP</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Adénocarcinome pulmonaire</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>24EM03352</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>24MH9794 RF</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>GP</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Centre Hospitalier de Mouscron</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Adénocarcinome lieberkühnien</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>20%</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Run LLM pipeline corrected + times saved
</commit_message>
<xml_diff>
--- a/out/metadata_gemma3_4B.xlsx
+++ b/out/metadata_gemma3_4B.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,17 +461,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Qualité du séquencage</t>
+          <t>Qualité du séquençage</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>% cellules</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Qualité du séquençage</t>
         </is>
       </c>
     </row>
@@ -508,10 +503,9 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>20%</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
+          <t>20</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -546,10 +540,9 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>10%</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -564,7 +557,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>CLP</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -584,10 +577,9 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>20%</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
+          <t>20</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -625,7 +617,6 @@
           <t>30</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -640,7 +631,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>OST</t>
+          <t>GP</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -653,15 +644,14 @@
           <t>PF2</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr">
         <is>
           <t>70</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Optimale</t>
         </is>
       </c>
     </row>
@@ -701,7 +691,6 @@
           <t>10</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -736,10 +725,9 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>10%</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -777,7 +765,6 @@
           <t>70</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -815,7 +802,6 @@
           <t>50</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -850,10 +836,9 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>30%</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr"/>
+          <t>30</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -891,7 +876,6 @@
           <t>50</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -906,7 +890,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>CLP</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -926,10 +910,9 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>50%</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr"/>
+          <t>50</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -964,10 +947,9 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>20%</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr"/>
+          <t>20</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Pre_download the models HF
</commit_message>
<xml_diff>
--- a/out/metadata_gemma3_4B.xlsx
+++ b/out/metadata_gemma3_4B.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>% cellules</t>
+          <t>% de cellules</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>OST</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>CLP</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">

</xml_diff>